<commit_message>
RPA Challenge in REframework
</commit_message>
<xml_diff>
--- a/SourceCode/2023/August2023/Charitha/RPA Challenge/challenge.xlsx
+++ b/SourceCode/2023/August2023/Charitha/RPA Challenge/challenge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherry\Documents\GitHub\RPA-Developer-in-30-Days\SourceCode\2023\August2023\Charitha\RPA Challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6F62D7-F8EC-4711-867E-8BD2A7A49C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DB0A6C-5D80-470B-B53B-83BB7A3FD6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -616,7 +616,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.08984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>